<commit_message>
feat: export excel tamamlandı
</commit_message>
<xml_diff>
--- a/exports/Blogs-export.xlsx
+++ b/exports/Blogs-export.xlsx
@@ -455,12 +455,32 @@
         <v>$collectionId</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" xml:space="preserve">
       <c r="A2" t="str">
         <v>Understanding QR Codes: A Complete Beginner's Guide</v>
       </c>
-      <c r="B2" t="str">
-        <v>&lt;h1&gt;Understanding QR Codes&lt;/h1&gt;&lt;p&gt;QR codes, or Quick Response codes, have become an integral part of our daily lives. These two-dimensional barcodes can store a wealth of information and are easily scannable with modern smartphones.&lt;/p&gt;&lt;h2&gt;What Are QR Codes?&lt;/h2&gt;&lt;p&gt;QR codes were invented in 1994 by Denso Wave, a Japanese automotive company. They were designed to track vehicles during manufacturing but have since evolved into a versatile tool used across various industries.&lt;/p&gt;&lt;h2&gt;How Do They Work?&lt;/h2&gt;&lt;p&gt;QR codes work by encoding data in a pattern of black squares arranged on a white background. When scanned, a QR code reader interprets this pattern and converts it into readable information.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Fast scanning capability&lt;/li&gt;&lt;li&gt;High error correction&lt;/li&gt;&lt;li&gt;Can store various data types&lt;/li&gt;&lt;/ul&gt;</v>
+      <c r="B2" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;Understanding QR Codes: A Complete Beginner's Guide&lt;/h2&gt;
+  &lt;p&gt;
+    QR codes, short for &lt;strong&gt;Quick Response codes&lt;/strong&gt;, are scannable square-shaped patterns that store information accessible through smartphones and scanning devices. Although they may look complex at first glance, QR codes operate on simple principles and offer countless practical uses. This guide provides a clear, beginner-friendly introduction to QR codes, their structure, and how they function in everyday life.
+  &lt;/p&gt;
+  &lt;p&gt;
+    A QR code is made up of black modules arranged on a white background. These modules encode data such as URLs, text, payment information, Wi-Fi credentials, or contact details. When scanned, the device interprets the pattern and instantly displays the corresponding content.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Beginners often wonder what makes QR codes different from traditional barcodes. The key advantage lies in their ability to store much more information thanks to their two-dimensional format. While barcodes can only hold data horizontally, QR codes store it both vertically and horizontally, allowing for significantly higher capacity and faster reading speeds.
+  &lt;/p&gt;
+  &lt;p&gt;
+    To scan a QR code, users simply open their smartphone camera or a QR scanning app. Most modern devices detect QR codes automatically, making the process quick and intuitive. Once scanned, the user is immediately directed to the embedded content.
+  &lt;/p&gt;
+  &lt;p&gt;
+    QR codes are widely used in marketing, education, retail, payments, and transportation. They provide a convenient way to access digital content without typing links or downloading additional materials.
+  &lt;/p&gt;
+  &lt;p&gt;
+    For beginners interested in creating QR codes, numerous free online generators make the process simple: enter your content, customize the design, test the code, and download it. Whether for business or personal use, QR codes offer a flexible, user-friendly tool for connecting the physical and digital worlds.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C2" t="str">
         <v>admin</v>
@@ -499,12 +519,32 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" xml:space="preserve">
       <c r="A3" t="str">
         <v>The Future of QR Technology in Marketing</v>
       </c>
-      <c r="B3" t="str">
-        <v>&lt;h1&gt;The Future of QR Technology in Marketing&lt;/h1&gt;&lt;p&gt;QR codes have transformed from simple tracking tools to powerful marketing instruments. Today's marketers leverage QR codes to create seamless customer experiences.&lt;/p&gt;&lt;h2&gt;Marketing Applications&lt;/h2&gt;&lt;p&gt;Modern businesses use QR codes for:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Product information and reviews&lt;/li&gt;&lt;li&gt;Loyalty programs&lt;/li&gt;&lt;li&gt;Event registration&lt;/li&gt;&lt;li&gt;Social media integration&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Trends to Watch&lt;/h2&gt;&lt;p&gt;The integration of QR codes with augmented reality and AI is creating new possibilities for interactive marketing campaigns.&lt;/p&gt;</v>
+      <c r="B3" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;The Future of QR Technology in Marketing&lt;/h2&gt;
+  &lt;p&gt;
+    As consumer behavior continues shifting toward mobile-first interactions, &lt;strong&gt;QR technology&lt;/strong&gt; is becoming a defining force in the future of digital marketing. What began as a simple tool for redirecting users to web pages has now evolved into a sophisticated ecosystem supporting automation, personalization, and immersive experiences.
+  &lt;/p&gt;
+  &lt;p&gt;
+    One of the most significant trends is the integration of QR codes with &lt;strong&gt;AI-powered personalization&lt;/strong&gt;. Marketers can now deliver tailored product recommendations, location-based offers, or dynamic content based on user behavior. This level of relevance enhances engagement and improves conversion rates dramatically.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Another development shaping the future of QR marketing is the rise of &lt;em&gt;augmented reality (AR)&lt;/em&gt;. By scanning a single code, consumers can visualize 3D products, explore virtual showrooms, or interact with promotional experiences that blur the line between digital and physical spaces. AR-enabled QR codes open doors to highly engaging, memorable campaigns.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Payment ecosystems will also grow more integrated with QR codes. Industries such as retail, hospitality, and transportation increasingly depend on contactless transactions. With the global expansion of digital wallets and banking apps, QR-based payments will continue to accelerate.
+  &lt;/p&gt;
+  &lt;p&gt;
+    In the broader marketing landscape, QR codes will serve as bridges between offline and online data. Detailed &lt;strong&gt;scan analytics&lt;/strong&gt; will help brands understand customer demographics, location patterns, and real-time engagement, enabling smarter campaign optimization.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Ultimately, the future of QR technology in marketing revolves around smarter interactivity, data-driven personalization, and immersive brand experiences. As innovation continues, QR codes will remain an essential tool for marketers seeking deeper connections with modern audiences.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C3" t="str">
         <v>admin</v>
@@ -543,12 +583,35 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" xml:space="preserve">
       <c r="A4" t="str">
         <v>Designing Beautiful QR Codes: Best Practices</v>
       </c>
-      <c r="B4" t="str">
-        <v>&lt;h1&gt;Designing Beautiful QR Codes&lt;/h1&gt;&lt;p&gt;Gone are the days of plain black and white QR codes. Modern design tools allow you to create stunning, branded QR codes that align with your visual identity.&lt;/p&gt;&lt;h2&gt;Design Principles&lt;/h2&gt;&lt;p&gt;When designing QR codes, consider:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Color schemes that maintain contrast&lt;/li&gt;&lt;li&gt;Logo integration without breaking functionality&lt;/li&gt;&lt;li&gt;Custom shapes and patterns&lt;/li&gt;&lt;li&gt;Error correction levels&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Tools and Resources&lt;/h2&gt;&lt;p&gt;Various online tools and APIs can help you create custom QR codes that are both functional and beautiful.&lt;/p&gt;</v>
+      <c r="B4" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;Designing Beautiful QR Codes: Best Practices&lt;/h2&gt;
+  &lt;p&gt;
+    Creating visually appealing and &lt;strong&gt;beautiful QR codes&lt;/strong&gt; is an effective way to improve user engagement and strengthen brand identity. While standard black-and-white QR codes function well, modern design trends encourage a balance between aesthetics and functionality. As customized QR codes become more common in marketing, packaging, and digital content, following established best practices ensures that your designs are both attractive and fully scannable.
+  &lt;/p&gt;
+  &lt;p&gt;
+    The first rule of beautiful QR design is maintaining &lt;strong&gt;high contrast&lt;/strong&gt;. Even when integrating brand colors, the foreground should remain significantly darker than the background. Failing to maintain contrast can lead to scanning errors, which frustrates users and reduces engagement.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Adding a logo is one of the most impactful ways to brand a QR code. Thanks to high error correction levels, designers can place a small logo at the center without affecting readability. However, the logo should never cover essential elements like the finder patterns located at the corners.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Shape customization is another creative technique. Modern QR generators allow for rounded modules, patterned corners, or stylized frames. These small adjustments can make your QR code feel more premium and on-brand. Still, it is important to avoid overly complex patterns that may confuse scanners.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Surrounding the QR code with a clear &lt;strong&gt;quiet zone&lt;/strong&gt;—a border with no design elements—is essential for smooth scanning. This empty space helps scanning devices identify where the QR code begins and ends.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Finally, incorporating a call-to-action such as “Scan to Shop” or “Scan for Details” increases scan rates significantly. When users understand what to expect, they are more likely to engage.
+  &lt;/p&gt;
+  &lt;p&gt;
+    By combining aesthetics with technical reliability, beautifully designed QR codes can elevate your marketing materials and deliver a powerful, professional impression.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C4" t="str">
         <v>admin</v>
@@ -587,12 +650,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" xml:space="preserve">
       <c r="A5" t="str">
         <v>QR Code Security: Protecting Your Data</v>
       </c>
-      <c r="B5" t="str">
-        <v>&lt;h1&gt;QR Code Security&lt;/h1&gt;&lt;p&gt;While QR codes are convenient, they can pose security risks if not implemented correctly. Understanding these risks is crucial for safe usage.&lt;/p&gt;&lt;h2&gt;Common Security Threats&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Malicious URL redirection&lt;/li&gt;&lt;li&gt;Phishing attacks&lt;/li&gt;&lt;li&gt;Data interception&lt;/li&gt;&lt;li&gt;Fake QR codes&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Best Practices&lt;/h2&gt;&lt;p&gt;To protect your users and data:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Always verify QR code sources&lt;/li&gt;&lt;li&gt;Use HTTPS for all redirects&lt;/li&gt;&lt;li&gt;Implement content validation&lt;/li&gt;&lt;li&gt;Regular security audits&lt;/li&gt;&lt;/ul&gt;</v>
+      <c r="B5" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;QR Code Security: Protecting Your Data&lt;/h2&gt;
+  &lt;p&gt;
+    As QR codes expand into payments, authentication, and personal data sharing, security has become a critical concern. While the code itself is harmless, the destination it leads to may expose users to fraud, phishing, or malware.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Secure implementations rely on &lt;strong&gt;encrypted HTTPS links&lt;/strong&gt; to prevent data interception. Dynamic QR codes add layers of control by enabling real-time monitoring and access restrictions.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Businesses must avoid embedding confidential information inside QR codes. Instead, they should store sensitive data securely on servers and use the QR code as a gateway.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Users should check for signs of tampering, verify URLs, and avoid scanning codes from unknown sources.
+  &lt;/p&gt;
+  &lt;p&gt;
+    By prioritizing security and awareness, QR codes remain a safe and reliable tool in the digital world.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C5" t="str">
         <v>admin</v>
@@ -631,12 +711,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" xml:space="preserve">
       <c r="A6" t="str">
         <v>The Evolution of QR Codes: From 1994 to Today</v>
       </c>
-      <c r="B6" t="str">
-        <v>&lt;h1&gt;The Evolution of QR Codes&lt;/h1&gt;&lt;p&gt;QR codes have come a long way since their invention in 1994. What started as an industrial tracking solution has become a global communication tool.&lt;/p&gt;&lt;h2&gt;Early Years (1994-2000)&lt;/h2&gt;&lt;p&gt;Initially used in automotive manufacturing, QR codes were primarily a B2B solution for inventory management.&lt;/p&gt;&lt;h2&gt;The Smartphone Revolution (2000-2010)&lt;/h2&gt;&lt;p&gt;The widespread adoption of smartphones with built-in cameras made QR codes accessible to consumers worldwide.&lt;/p&gt;&lt;h2&gt;Modern Era (2010-Present)&lt;/h2&gt;&lt;p&gt;Today, QR codes are everywhere - from restaurant menus to payment systems, transforming how we interact with digital content.&lt;/p&gt;</v>
+      <c r="B6" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;The Evolution of QR Codes: From 1994 to Today&lt;/h2&gt;
+  &lt;p&gt;
+    Since their creation in 1994 by Denso Wave, QR codes have undergone a remarkable transformation. Initially designed to track automotive components, they quickly expanded into consumer markets due to their speed and high data capacity.
+  &lt;/p&gt;
+  &lt;p&gt;
+    The rise of smartphones unlocked a new era of QR technology. With built-in scanners and high-resolution cameras, users could instantly access websites and digital content.
+  &lt;/p&gt;
+  &lt;p&gt;
+    During the COVID-19 pandemic, QR codes experienced unprecedented global adoption in payments, health passes, menus, and remote access services.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Today, QR codes integrate with AI, biometrics, AR, and IoT systems, continuing to revolutionize digital connectivity.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Their evolution reflects the ongoing shift toward contactless, efficient, and user-friendly interactions.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C6" t="str">
         <v>admin</v>
@@ -675,12 +772,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" xml:space="preserve">
       <c r="A7" t="str">
         <v>QR Codes in Everyday Life: Practical Applications</v>
       </c>
-      <c r="B7" t="str">
-        <v>&lt;h1&gt;QR Codes in Everyday Life&lt;/h1&gt;&lt;p&gt;QR codes have seamlessly integrated into our daily routines, making many tasks more convenient and efficient.&lt;/p&gt;&lt;h2&gt;Common Uses&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Restaurant menus and ordering&lt;/li&gt;&lt;li&gt;Public transportation tickets&lt;/li&gt;&lt;li&gt;Event check-ins&lt;/li&gt;&lt;li&gt;Wi-Fi network sharing&lt;/li&gt;&lt;li&gt;Contact information exchange&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Lifestyle Benefits&lt;/h2&gt;&lt;p&gt;The convenience of QR codes has transformed how we interact with services, reducing wait times and improving user experiences across various industries.&lt;/p&gt;</v>
+      <c r="B7" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;QR Codes in Everyday Life: Practical Applications&lt;/h2&gt;
+  &lt;p&gt;
+    From payments to education, &lt;strong&gt;QR codes&lt;/strong&gt; have become a seamless part of modern routines. Their simplicity and versatility enable countless practical uses across daily activities.
+  &lt;/p&gt;
+  &lt;p&gt;
+    QR codes are widely used in &lt;strong&gt;restaurants&lt;/strong&gt; for digital menus, reducing printing needs and allowing instant updates. In transportation, they simplify ticketing and boarding processes.
+  &lt;/p&gt;
+  &lt;p&gt;
+    In workplaces, QR codes support inventory tracking, employee check-ins, and equipment logs. They also play an essential role in healthcare by linking patients to digital records, appointment systems, and prescription details.
+  &lt;/p&gt;
+  &lt;p&gt;
+    QR codes even help enhance safety by enabling contactless access control and emergency information sharing.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Their convenience makes them a lasting tool in everyday life.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C7" t="str">
         <v>admin</v>
@@ -719,12 +833,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" xml:space="preserve">
       <c r="A8" t="str">
         <v>QR Code Types: Static vs Dynamic Explained</v>
       </c>
-      <c r="B8" t="str">
-        <v>&lt;h1&gt;QR Code Types: Static vs Dynamic&lt;/h1&gt;&lt;p&gt;Not all QR codes are created equal. Understanding the difference between static and dynamic QR codes is essential for choosing the right solution.&lt;/p&gt;&lt;h2&gt;Static QR Codes&lt;/h2&gt;&lt;p&gt;Static QR codes contain fixed information that cannot be changed once generated. They're perfect for:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Wi-Fi passwords&lt;/li&gt;&lt;li&gt;Contact information&lt;/li&gt;&lt;li&gt;Simple URLs&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Dynamic QR Codes&lt;/h2&gt;&lt;p&gt;Dynamic QR codes can be edited after creation, allowing you to:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Update destination URLs&lt;/li&gt;&lt;li&gt;Track scan analytics&lt;/li&gt;&lt;li&gt;Change content without reprinting&lt;/li&gt;&lt;/ul&gt;</v>
+      <c r="B8" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;QR Code Types: Static vs Dynamic Explained&lt;/h2&gt;
+  &lt;p&gt;
+    QR codes come in two primary forms: &lt;strong&gt;static&lt;/strong&gt; and &lt;strong&gt;dynamic&lt;/strong&gt;. Understanding the difference is crucial for selecting the right type for your project.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Static QR codes contain fixed, unchangeable information. Once generated, their content cannot be updated. They are ideal for permanent uses such as contact details, Wi-Fi passwords, or printed documents.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Dynamic QR codes, however, allow the destination link to be updated at any time. They support advanced features like analytics, A/B testing, password protection, and expiration settings.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Businesses prefer dynamic QR codes for marketing campaigns due to their flexibility and performance tracking capabilities.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Both types serve unique purposes, and choosing the right one ensures efficiency and long-term reliability.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C8" t="str">
         <v>admin</v>
@@ -763,12 +894,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" xml:space="preserve">
       <c r="A9" t="str">
         <v>Innovative QR Code Uses in 2024</v>
       </c>
-      <c r="B9" t="str">
-        <v>&lt;h1&gt;Innovative QR Code Uses in 2024&lt;/h1&gt;&lt;p&gt;The QR code landscape continues to evolve with innovative applications emerging across industries.&lt;/p&gt;&lt;h2&gt;Emerging Trends&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;AR-enhanced QR experiences&lt;/li&gt;&lt;li&gt;Blockchain-based verification&lt;/li&gt;&lt;li&gt;IoT device configuration&lt;/li&gt;&lt;li&gt;Healthcare patient portals&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Industry Innovations&lt;/h2&gt;&lt;p&gt;From retail to healthcare, businesses are finding creative ways to leverage QR technology for improved customer experiences and operational efficiency.&lt;/p&gt;</v>
+      <c r="B9" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;Innovative QR Code Uses in 2024&lt;/h2&gt;
+  &lt;p&gt;
+    In 2024, QR codes have evolved far beyond simple URL links. Their integration with technologies like &lt;strong&gt;AI&lt;/strong&gt;, &lt;em&gt;augmented reality&lt;/em&gt;, biometrics, and IoT devices has opened new possibilities across industries.
+  &lt;/p&gt;
+  &lt;p&gt;
+    One of the most exciting developments is QR-driven smart packaging. Consumers can scan codes to view product authenticity, nutritional data, recycling instructions, or supply chain traceability.
+  &lt;/p&gt;
+  &lt;p&gt;
+    In transportation, QR codes support ticketing, identity verification, and real-time updates, improving efficiency and user convenience.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Hospitality and retail sectors are using QR codes for personalized recommendations, loyalty rewards, and immersive shopping experiences.
+  &lt;/p&gt;
+  &lt;p&gt;
+    As innovation accelerates, QR codes continue to redefine everyday interactions and digital connectivity.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C9" t="str">
         <v>admin</v>
@@ -807,12 +955,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" xml:space="preserve">
       <c r="A10" t="str">
         <v>Creating Branded QR Codes: A Design Guide</v>
       </c>
-      <c r="B10" t="str">
-        <v>&lt;h1&gt;Creating Branded QR Codes&lt;/h1&gt;&lt;p&gt;Branded QR codes help maintain visual consistency while providing the functionality of traditional QR codes.&lt;/p&gt;&lt;h2&gt;Design Elements&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Brand colors and gradients&lt;/li&gt;&lt;li&gt;Logo placement strategies&lt;/li&gt;&lt;li&gt;Custom frame designs&lt;/li&gt;&lt;li&gt;Pattern customization&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Implementation Tips&lt;/h2&gt;&lt;p&gt;When creating branded QR codes, always test scanability across different devices and lighting conditions to ensure optimal performance.&lt;/p&gt;</v>
+      <c r="B10" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;Creating Branded QR Codes: A Design Guide&lt;/h2&gt;
+  &lt;p&gt;
+    As businesses embrace more personalized digital experiences, &lt;strong&gt;branded QR codes&lt;/strong&gt; have become a key visual asset. By customizing color, shape, and logos, brands can transform standard QR codes into powerful marketing tools that strengthen recognition and boost engagement.
+  &lt;/p&gt;
+  &lt;p&gt;
+    The most important rule is maintaining high contrast between the code and the background. Dark foreground colors paired with light backgrounds ensure reliable scanning across devices.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Adding logos inside the center of the QR code is a popular trend. With proper error correction, the code remains scannable even with a logo overlay. Designers should avoid covering critical patterns like finder markers.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Creative frames, call-to-action texts, and stylistic elements also help draw user attention. A well-designed branded QR code looks professional, visually appealing, and instantly recognizable.
+  &lt;/p&gt;
+  &lt;p&gt;
+    When done correctly, branded QR codes enhance marketing outcomes while maintaining full technical functionality.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C10" t="str">
         <v>admin</v>
@@ -851,12 +1016,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" xml:space="preserve">
       <c r="A11" t="str">
         <v>QR Code Encryption and Privacy Protection</v>
       </c>
-      <c r="B11" t="str">
-        <v>&lt;h1&gt;QR Code Encryption and Privacy Protection&lt;/h1&gt;&lt;p&gt;Protecting user data and privacy is paramount when implementing QR code solutions in sensitive applications.&lt;/p&gt;&lt;h2&gt;Encryption Methods&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;End-to-end encryption&lt;/li&gt;&lt;li&gt;Token-based authentication&lt;/li&gt;&lt;li&gt;Time-limited access codes&lt;/li&gt;&lt;li&gt;Secure data transmission&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Privacy Best Practices&lt;/h2&gt;&lt;p&gt;Implementing proper privacy controls ensures that user data remains protected while maintaining the convenience of QR code technology.&lt;/p&gt;</v>
+      <c r="B11" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;QR Code Encryption and Privacy Protection&lt;/h2&gt;
+  &lt;p&gt;
+    With the rise of QR code–based payments, authentication, and data sharing, &lt;strong&gt;privacy protection&lt;/strong&gt; and security have become top priorities. While QR codes themselves are simple containers, the data they link to must be protected through robust encryption and access control measures.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Secure QR systems typically use &lt;strong&gt;HTTPS encryption&lt;/strong&gt; to safeguard data in transit. Additionally, dynamic QR codes allow businesses to manage content on secure servers, reducing risks associated with static URLs.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Advanced implementations may include &lt;em&gt;tokenization&lt;/em&gt;, password protection, or single-use QR codes to prevent unauthorized access. These are particularly valuable in settings such as banking, healthcare, and identity verification.
+  &lt;/p&gt;
+  &lt;p&gt;
+    To protect privacy, organizations must avoid embedding sensitive data directly inside QR codes. Instead, they should store such data on secure servers and link it via encrypted channels.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Prioritizing encryption and privacy ensures that QR codes remain a trusted tool for digital interactions.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C11" t="str">
         <v>admin</v>
@@ -895,12 +1077,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" xml:space="preserve">
       <c r="A12" t="str">
         <v>The Technical Specifications of QR Codes</v>
       </c>
-      <c r="B12" t="str">
-        <v>&lt;h1&gt;Technical Specifications of QR Codes&lt;/h1&gt;&lt;p&gt;Understanding the technical foundation of QR codes helps in optimizing their implementation for specific use cases.&lt;/p&gt;&lt;h2&gt;Data Capacity&lt;/h2&gt;&lt;p&gt;QR codes can store different amounts of data depending on their version and error correction level:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Numeric: up to 7,089 characters&lt;/li&gt;&lt;li&gt;Alphanumeric: up to 4,296 characters&lt;/li&gt;&lt;li&gt;Binary: up to 2,953 bytes&lt;/li&gt;&lt;li&gt;Kanji: up to 1,817 characters&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Error Correction Levels&lt;/h2&gt;&lt;p&gt;QR codes support four error correction levels (L, M, Q, H) that determine how much damage the code can sustain while remaining scannable.&lt;/p&gt;</v>
+      <c r="B12" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;The Technical Specifications of QR Codes&lt;/h2&gt;
+  &lt;p&gt;
+    QR codes operate based on a precise set of &lt;strong&gt;technical specifications&lt;/strong&gt; defined under ISO/IEC 18004. These specifications ensure that QR codes remain consistent, scannable, and interoperable across devices and platforms worldwide.
+  &lt;/p&gt;
+  &lt;p&gt;
+    A QR code consists of modules arranged in a square grid. Key components include finder patterns, alignment patterns, timing patterns, and data modules. Each serves a purpose in ensuring accurate scanning.
+  &lt;/p&gt;
+  &lt;p&gt;
+    QR codes also support four error correction levels—L, M, Q, and H—allowing data to be reconstructed even when parts of the code are damaged. Higher correction levels increase scan reliability but reduce available data capacity.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Encoding formats include numeric, alphanumeric, byte, and Kanji modes. These variations enable QR codes to store diverse types of information, from URLs and text to structured data.
+  &lt;/p&gt;
+  &lt;p&gt;
+    The combination of these specifications forms the backbone of modern QR code functionality, enabling their widespread use across industries.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C12" t="str">
         <v>admin</v>
@@ -939,12 +1138,43 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" xml:space="preserve">
       <c r="A13" t="str">
         <v>QR Codes for Event Management</v>
       </c>
-      <c r="B13" t="str">
-        <v>&lt;h1&gt;QR Codes for Event Management&lt;/h1&gt;&lt;p&gt;Event organizers are increasingly using QR codes to simplify registration and enhance attendee experiences.&lt;/p&gt;&lt;h2&gt;Event Applications&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Quick registration and check-in&lt;/li&gt;&lt;li&gt;Digital ticket validation&lt;/li&gt;&lt;li&gt;Networking contact exchange&lt;/li&gt;&lt;li&gt;Feedback collection&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Benefits&lt;/h2&gt;&lt;p&gt;QR codes reduce wait times, minimize errors, and provide valuable data insights for event organizers.&lt;/p&gt;</v>
+      <c r="B13" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;p&gt;
+The use of &lt;strong&gt;QR codes for event management&lt;/strong&gt; has rapidly transformed how organizers handle guest registration, ticketing, crowd control, and post-event analytics. As events continue shifting toward digital-first solutions, &lt;strong&gt;QR-based workflows&lt;/strong&gt; offer unmatched levels of &lt;em&gt;speed&lt;/em&gt;, &lt;em&gt;accuracy&lt;/em&gt;, and &lt;em&gt;automation&lt;/em&gt;. From small workshops to international conferences, QR technology enables a seamless experience for both event organizers and attendees.
+&lt;/p&gt;
+&lt;p&gt;
+One of the strongest advantages of using &lt;strong&gt;QR codes for tickets and entry management&lt;/strong&gt; is the significant reduction in wait times at entrance points. Traditional paper tickets or manual check-in systems often cause delays and create long queues. In contrast, QR codes allow staff to scan attendees within seconds using any compatible mobile device. This not only speeds up the process but also enhances &lt;strong&gt;operational efficiency&lt;/strong&gt; and improves the overall visitor experience.
+&lt;/p&gt;
+&lt;p&gt;
+For event organizers, utilizing &lt;strong&gt;dynamic QR codes&lt;/strong&gt; provides even greater flexibility. Because dynamic codes can be updated in real time, organizers can modify attendee information, adjust schedules, or update ticket types without having to reissue new codes. This is especially useful for multi-day events or events with multiple access tiers. Additionally, dynamic QR codes can embed advanced tracking parameters, enabling more detailed performance analytics.
+&lt;/p&gt;
+&lt;p&gt;
+Event marketers also benefit from integrating &lt;strong&gt;QR codes into promotional materials&lt;/strong&gt;. Whether displayed on posters, social media posts, emails, or print advertisements, QR codes make it effortless for potential attendees to access event pages, buy tickets, or register instantly. This reduces friction in the customer journey and often leads to higher conversion rates. To optimize results, organizers can design &lt;u&gt;visually appealing&lt;/u&gt; and &lt;strong&gt;branded QR codes&lt;/strong&gt; that match the event’s theme and enhance brand recognition.
+&lt;/p&gt;
+&lt;p&gt;
+Another critical benefit of QR codes in event management is their ability to support &lt;strong&gt;contactless interactions&lt;/strong&gt;. In recent years, the demand for touch-free solutions has increased rapidly across industries, including the event sector. QR-based solutions allow attendees to access maps, schedules, speaker information, and menus without needing physical brochures or printed materials. This not only reduces operational costs but also supports sustainability by minimizing paper waste.
+&lt;/p&gt;
+&lt;p&gt;
+Moreover, QR codes enable powerful &lt;strong&gt;real-time data collection&lt;/strong&gt;. Every scan can provide insight into attendee behavior, such as peak entry times, session popularity, or engagement levels with exhibitors. Organizers can use this data to optimize event flow, allocate staff more efficiently, or improve booth placement. After the event, these analytics serve as high-value inputs for planning future events, enhancing ROI, and improving attendee satisfaction.
+&lt;/p&gt;
+&lt;p&gt;
+Security is another essential aspect where QR codes contribute significantly. When paired with backend validation systems, &lt;strong&gt;QR-based tickets&lt;/strong&gt; help reduce fraud by ensuring that each code is unique and cannot be duplicated easily. Event organizers can also control access rights, marking codes as used after they’re scanned and blocking unauthorized re-entry attempts. For high-profile or paid events, this level of security is crucial.
+&lt;/p&gt;
+&lt;p&gt;
+In addition to ticketing and registration, QR codes support a variety of &lt;strong&gt;in-event engagement activities&lt;/strong&gt;. Organizers can set up QR codes for surveys, live polls, networking features, and gamification elements that encourage greater participant interaction. Exhibitors at trade shows can use QR codes to provide brochures, product demos, or contact information, reducing the need for printed marketing materials.
+&lt;/p&gt;
+&lt;p&gt;
+Looking ahead, the role of &lt;strong&gt;QR codes in event management&lt;/strong&gt; will continue expanding as technology evolves. With AI-driven analytics, NFC integrations, and personalized QR-based experiences, event planners can look forward to even more sophisticated tools that streamline event operations. In a competitive digital landscape, adopting innovative QR solutions is no longer optional—it is a crucial strategy for creating engaging, efficient, and memorable events.
+&lt;/p&gt;
+&lt;p&gt;
+In summary, the integration of QR codes into event workflows offers a wide range of benefits including &lt;strong&gt;efficiency&lt;/strong&gt;, &lt;strong&gt;security&lt;/strong&gt;, &lt;strong&gt;data insights&lt;/strong&gt;, and &lt;strong&gt;improved attendee engagement&lt;/strong&gt;. By combining smart design, dynamic functionality, and strategic placement, QR codes can significantly elevate the success of any event. As organizations continue to seek modern, scalable, and cost-effective tools, QR-based event management stands out as one of the most powerful solutions available today.
+&lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C13" t="str">
         <v>admin</v>
@@ -983,12 +1213,44 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" xml:space="preserve">
       <c r="A14" t="str">
         <v>How to Generate QR Codes: A Step-by-Step Tutorial</v>
       </c>
-      <c r="B14" t="str">
-        <v>&lt;h1&gt;How to Generate QR Codes&lt;/h1&gt;&lt;p&gt;Creating QR codes is easier than ever with modern tools and APIs. This tutorial covers multiple approaches.&lt;/p&gt;&lt;h2&gt;Online Generators&lt;/h2&gt;&lt;p&gt;Simple web-based tools allow quick QR code generation without technical knowledge.&lt;/p&gt;&lt;h2&gt;API Integration&lt;/h2&gt;&lt;p&gt;For developers, QR code APIs provide programmatic control and customization options.&lt;/p&gt;&lt;h2&gt;Best Practices&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Choose appropriate error correction level&lt;/li&gt;&lt;li&gt;Test before deployment&lt;/li&gt;&lt;li&gt;Consider size and placement&lt;/li&gt;&lt;li&gt;Ensure good contrast&lt;/li&gt;&lt;/ul&gt;</v>
+      <c r="B14" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;How to Generate QR Codes: A Step-by-Step Tutorial&lt;/h2&gt;
+  &lt;p&gt;
+    Creating a QR code is easier than ever, thanks to modern tools and intuitive platforms. Whether you're building one for marketing, payments, or educational purposes, following a structured process ensures your code is both functional and visually appealing. This guide explains how to generate a QR code effectively while optimizing it for user engagement.
+  &lt;/p&gt;
+  &lt;h3&gt;1. Define Your Purpose&lt;/h3&gt;
+  &lt;p&gt;
+    Start by identifying what your QR code will link to. Common options include &lt;strong&gt;URLs&lt;/strong&gt;, PDFs, contact information, payment links, app downloads, or Wi-Fi credentials. Choosing the right type ensures accuracy and a seamless user experience.
+  &lt;/p&gt;
+  &lt;h3&gt;2. Select a QR Code Generator&lt;/h3&gt;
+  &lt;p&gt;
+    Many platforms offer QR code creation services—from free browser tools to advanced dynamic QR solutions. Look for features such as branding options, analytics, password protection, and editable destinations.
+  &lt;/p&gt;
+  &lt;h3&gt;3. Enter Your Content&lt;/h3&gt;
+  &lt;p&gt;
+    Once you've selected a generator, input the destination. For dynamic QR codes, you can update the content later, making them ideal for marketing campaigns and long-term use.
+  &lt;/p&gt;
+  &lt;h3&gt;4. Customize the Design&lt;/h3&gt;
+  &lt;p&gt;
+    To boost recognition, add &lt;strong&gt;brand colors&lt;/strong&gt;, logos, and distinctive shapes. Ensure contrast remains high to keep the QR code scannable. Avoid overly complex patterns that could confuse scanners.
+  &lt;/p&gt;
+  &lt;h3&gt;5. Test the QR Code&lt;/h3&gt;
+  &lt;p&gt;
+    Before distributing, test the code across multiple devices and lighting environments. This step ensures reliable scanning and prevents user frustration.
+  &lt;/p&gt;
+  &lt;h3&gt;6. Download and Deploy&lt;/h3&gt;
+  &lt;p&gt;
+    Export your QR code in the appropriate format such as PNG, SVG, or PDF. Then place it on packaging, websites, brochures, or digital ads.
+  &lt;/p&gt;
+  &lt;p&gt;
+    By following these steps, you can generate QR codes that are practical, professional, and ready for real-world use.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C14" t="str">
         <v>admin</v>
@@ -1027,12 +1289,29 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" xml:space="preserve">
       <c r="A15" t="str">
         <v>QR Codes in E-Commerce: Trends and Opportunities</v>
       </c>
-      <c r="B15" t="str">
-        <v>&lt;h1&gt;QR Codes in E-Commerce&lt;/h1&gt;&lt;p&gt;E-commerce businesses are finding innovative ways to integrate QR codes into their customer journey.&lt;/p&gt;&lt;h2&gt;Current Applications&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Product information and reviews&lt;/li&gt;&lt;li&gt;Mobile payment solutions&lt;/li&gt;&lt;li&gt;Loyalty program integration&lt;/li&gt;&lt;li&gt;Social media sharing&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Future Opportunities&lt;/h2&gt;&lt;p&gt;As technology evolves, QR codes will play an even larger role in bridging online and offline shopping experiences.&lt;/p&gt;</v>
+      <c r="B15" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;h2&gt;QR Codes in E-Commerce: Trends and Opportunities&lt;/h2&gt;
+  &lt;p&gt;
+    The rise of mobile-first shopping has positioned &lt;strong&gt;QR codes&lt;/strong&gt; as a powerful tool in modern e-commerce. These codes bridge the gap between offline and online retail, allowing customers to instantly access product pages, discounts, reviews, and personalized offers. As consumer behavior shifts toward convenience and speed, QR codes have become a strategic asset for brands seeking to enhance engagement and conversions.
+  &lt;/p&gt;
+  &lt;p&gt;
+    One of the most notable trends is the use of &lt;strong&gt;QR codes in packaging&lt;/strong&gt;. Brands now embed scannable codes on boxes, labels, and instruction manuals to provide product details, troubleshooting guides, or subscription reorders. This not only improves customer experience but also reduces support costs and boosts brand loyalty.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Another growing opportunity is the integration of QR codes in &lt;strong&gt;social commerce&lt;/strong&gt;. Platforms like Instagram, TikTok, and YouTube enable creators and businesses to link codes within videos and posts, making it easier for buyers to complete purchases instantly. This trend fuels impulse buying and creates a seamless journey from discovery to checkout.
+  &lt;/p&gt;
+  &lt;p&gt;
+    QR codes are also reshaping physical retail. In-store shoppers can scan codes for stock availability, promotional deals, or virtual try-ons. The combination of QR code data and analytics helps businesses refine marketing strategies, optimize inventory, and understand customer preferences.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Looking ahead, QR codes will continue to revolutionize e-commerce by supporting advanced technologies like &lt;em&gt;augmented reality&lt;/em&gt;, &lt;strong&gt;smart packaging&lt;/strong&gt;, and personalized customer journeys. Brands that adopt QR-driven experiences will gain a competitive edge in the evolving digital marketplace.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C15" t="str">
         <v>admin</v>
@@ -1071,12 +1350,47 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" xml:space="preserve">
       <c r="A16" t="str">
         <v>Color Psychology in QR Code Design</v>
       </c>
-      <c r="B16" t="str">
-        <v>&lt;h1&gt;Color Psychology in QR Code Design&lt;/h1&gt;&lt;p&gt;Color selection in QR code design goes beyond aesthetics - it can influence user behavior and brand perception.&lt;/p&gt;&lt;h2&gt;Color Impact&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Brand recognition and recall&lt;/li&gt;&lt;li&gt;Emotional response triggers&lt;/li&gt;&lt;li&gt;Scanability considerations&lt;/li&gt;&lt;li&gt;Cultural color associations&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Design Balance&lt;/h2&gt;&lt;p&gt;Successful QR code design balances visual appeal with functional requirements, ensuring both brand alignment and reliable scanning.&lt;/p&gt;</v>
+      <c r="B16" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;p&gt;
+    While QR codes are traditionally black and white, modern brands increasingly use color to improve visual appeal, brand recognition, and scan engagement. Understanding the principles of &lt;strong&gt;color psychology&lt;/strong&gt; and technical constraints is crucial for creating QR codes that are both aesthetically pleasing and highly functional.
+  &lt;/p&gt;
+  &lt;h2&gt;The Impact of Color on User Behavior&lt;/h2&gt;
+  &lt;p&gt;
+    Colors influence emotions and decision-making. For example, &lt;strong&gt;blue&lt;/strong&gt; conveys trust and security, making it ideal for financial apps, while &lt;strong&gt;green&lt;/strong&gt; represents sustainability and health. When applied correctly, color can enhance the visibility and perception of QR codes, increasing the likelihood of user interaction.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Brands often incorporate their signature colors to strengthen identity and create a seamless user experience. A QR code that matches marketing materials feels more intentional and professional, which increases credibility and scanning rates.
+  &lt;/p&gt;
+  &lt;h2&gt;Design Principles for Colored QR Codes&lt;/h2&gt;
+  &lt;p&gt;
+    Although creative freedom is allowed, certain rules must be followed to maintain scannability. The most important guideline is ensuring high &lt;strong&gt;contrast&lt;/strong&gt; between the foreground (QR pattern) and the background. Dark foreground colors—such as navy, forest green, or maroon—work best when paired with light backgrounds.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Designers should avoid overly complex gradients or low-contrast palettes, as they may reduce readability. It is also important to maintain clear quiet zones (empty space around the code) and avoid distorting the pattern with unnecessary decorations.
+  &lt;/p&gt;
+  &lt;h2&gt;Emotional and Brand-Focused Color Choices&lt;/h2&gt;
+  &lt;p&gt;
+    Selecting colors based on psychological impact can strengthen user engagement. For example:
+    &lt;ul&gt;
+      &lt;li&gt;&lt;strong&gt;Red&lt;/strong&gt;: urgency, excitement, energy&lt;/li&gt;
+      &lt;li&gt;&lt;strong&gt;Yellow&lt;/strong&gt;: optimism, warmth, attention&lt;/li&gt;
+      &lt;li&gt;&lt;strong&gt;Purple&lt;/strong&gt;: creativity, luxury, innovation&lt;/li&gt;
+    &lt;/ul&gt;
+    Matching these color associations to campaign goals can boost the effectiveness of QR code marketing strategies.
+  &lt;/p&gt;
+  &lt;h2&gt;Balancing Creativity and Function&lt;/h2&gt;
+  &lt;p&gt;
+    While colored QR codes provide branding opportunities, functionality must always remain the priority. Testing the code across multiple devices, lighting conditions, and print formats is essential to ensure reliable scanning.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Ultimately, a well-designed colored QR code blends art and utility. By leveraging color psychology and adhering to technical best practices, businesses can create visually compelling and user-friendly QR code experiences that enhance engagement and leave a lasting impression.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C16" t="str">
         <v>admin</v>
@@ -1115,12 +1429,44 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" xml:space="preserve">
       <c r="A17" t="str">
         <v>Preventing QR Code Fraud and Scams</v>
       </c>
-      <c r="B17" t="str">
-        <v>&lt;h1&gt;Preventing QR Code Fraud and Scams&lt;/h1&gt;&lt;p&gt;As QR codes become more prevalent, so do the security risks. Understanding these threats is crucial for safe implementation.&lt;/p&gt;&lt;h2&gt;Common Scams&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Fake QR code overlays&lt;/li&gt;&lt;li&gt;Malicious URL redirection&lt;/li&gt;&lt;li&gt;Phishing attempts&lt;/li&gt;&lt;li&gt;Data harvesting schemes&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Protection Strategies&lt;/h2&gt;&lt;p&gt;Implementing verification processes, user education, and technical safeguards can significantly reduce fraud risks.&lt;/p&gt;</v>
+      <c r="B17" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+  &lt;p&gt;
+    As QR codes become more common in everyday interactions—from payments to event check-ins—their popularity has also attracted cybercriminals. &lt;strong&gt;QR code fraud&lt;/strong&gt; is a growing threat, enabling attackers to redirect users to malicious websites, steal personal information, or perform unauthorized transactions. Understanding how these scams work and implementing preventive measures is essential for both businesses and consumers.
+  &lt;/p&gt;
+  &lt;h2&gt;How QR Code Scams Work&lt;/h2&gt;
+  &lt;p&gt;
+    Fraudsters typically replace legitimate QR codes with counterfeit ones, either physically or digitally. When scanned, these malicious codes may lead to phishing pages, fake payment portals, or malware downloads. Because QR codes appear simple and harmless, many users scan them without verifying the source, creating an ideal opportunity for exploitation.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Another common tactic is the use of &lt;strong&gt;QRishing&lt;/strong&gt;—a combination of QR codes and phishing. Attackers embed harmful URLs inside visually normal-looking codes, tricking users into revealing sensitive data. With the rise of touchless payments and digital menus, such scams have increased significantly.
+  &lt;/p&gt;
+  &lt;h2&gt;Best Practices for Prevention&lt;/h2&gt;
+  &lt;p&gt;
+    Organizations should implement several security measures, including:
+    &lt;ul&gt;
+      &lt;li&gt;&lt;strong&gt;Using HTTPS&lt;/strong&gt; for all QR destinations&lt;/li&gt;
+      &lt;li&gt;Adding &lt;strong&gt;brand logos&lt;/strong&gt; or visual identifiers&lt;/li&gt;
+      &lt;li&gt;Applying &lt;strong&gt;tamper-resistant stickers&lt;/strong&gt; for printed codes&lt;/li&gt;
+      &lt;li&gt;Using &lt;u&gt;dynamic QR codes&lt;/u&gt; with tracking and verification&lt;/li&gt;
+    &lt;/ul&gt;
+    These steps help ensure authenticity and reduce the likelihood of code replacement.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Consumers also play a crucial role in preventing scams. Before scanning, users should check whether a QR code appears altered, damaged, or suspiciously placed. Additionally, mobile devices should be equipped with security software capable of detecting malicious URLs.
+  &lt;/p&gt;
+  &lt;h2&gt;The Role of Dynamic QR Codes&lt;/h2&gt;
+  &lt;p&gt;
+    Dynamic QR codes offer an added layer of protection by allowing the destination URL to be managed and monitored through a secure server. Businesses can update links in real time, track suspicious activity, and disable compromised codes instantly. This makes dynamic systems more resilient compared to static QR codes.
+  &lt;/p&gt;
+  &lt;p&gt;
+    By staying vigilant and applying robust verification methods, organizations and users alike can significantly reduce their exposure to QR code fraud. Prioritizing security ensures that QR code interactions remain safe, reliable, and beneficial across industries.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C17" t="str">
         <v>admin</v>
@@ -1159,12 +1505,37 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" xml:space="preserve">
       <c r="A18" t="str">
         <v>QR Code Standards: ISO and Industry Guidelines</v>
       </c>
-      <c r="B18" t="str">
-        <v>&lt;h1&gt;QR Code Standards&lt;/h1&gt;&lt;p&gt;QR codes are governed by international standards that ensure compatibility and reliability across platforms.&lt;/p&gt;&lt;h2&gt;ISO Standards&lt;/h2&gt;&lt;p&gt;The ISO/IEC 18004 standard defines QR code specifications, ensuring consistent implementation worldwide.&lt;/p&gt;&lt;h2&gt;Industry Guidelines&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Data encoding standards&lt;/li&gt;&lt;li&gt;Error correction requirements&lt;/li&gt;&lt;li&gt;Size and placement recommendations&lt;/li&gt;&lt;li&gt;Accessibility considerations&lt;/li&gt;&lt;/ul&gt;</v>
+      <c r="B18" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article&gt;
+    &lt;p&gt;
+    The rapid growth of &lt;strong&gt;QR codes&lt;/strong&gt; across industries has made standardization essential for ensuring consistency, reliability, and global interoperability. As QR codes become a core part of payment systems, marketing campaigns, logistics operations, and product authentication, organizations must follow established &lt;strong&gt;ISO standards&lt;/strong&gt; and industry guidelines to deliver secure and efficient user experiences.
+  &lt;/p&gt;
+  &lt;h2&gt;ISO Standards for QR Codes&lt;/h2&gt;
+  &lt;p&gt;
+    The most important regulation governing QR codes is the &lt;strong&gt;ISO/IEC 18004&lt;/strong&gt; standard. This global standard defines the structure, encoding methods, symbol versions, error correction levels, and readability requirements for QR codes. It ensures that QR codes created by different software and scanned by various devices remain compatible across borders and platforms.
+  &lt;/p&gt;
+  &lt;p&gt;
+    ISO/IEC 18004 also outlines four error correction levels—L, M, Q, and H—allowing QR codes to remain readable even if they are partially damaged or obscured. Selecting the appropriate correction level is critical for industries such as &lt;strong&gt;manufacturing&lt;/strong&gt; and &lt;strong&gt;healthcare&lt;/strong&gt;, where reliability and accuracy are mandatory.
+  &lt;/p&gt;
+  &lt;h2&gt;Industry-Specific Guidelines&lt;/h2&gt;
+  &lt;p&gt;
+    Beyond ISO standards, many industries have their own QR code implementation guidelines. For example, the &lt;strong&gt;GS1 organization&lt;/strong&gt; provides global standards for supply chain and retail QR codes, enabling product traceability and efficient inventory management. GS1 Digital Link standard connects QR codes to detailed product information, enhancing transparency for consumers.
+  &lt;/p&gt;
+  &lt;p&gt;
+    In the financial sector, QR codes must comply with &lt;strong&gt;EMVCo specifications&lt;/strong&gt;. These rules ensure secure and interoperable mobile payment experiences worldwide, preventing fraud and enabling cross-border transactions. Today, most major payment providers—including Visa, Mastercard, and regional wallets—adhere to EMVCo QR code guidelines.
+  &lt;/p&gt;
+  &lt;h2&gt;Why Standards Matter&lt;/h2&gt;
+  &lt;p&gt;
+    Standardized QR codes offer several benefits. They ensure &lt;strong&gt;global readability&lt;/strong&gt;, minimize scanning errors, support secure transactions, and help brands maintain consistent quality across digital interactions. As QR codes continue to expand into transportation, advertising, and authentication, compliance with ISO and industry guidelines becomes even more important for long-term scalability.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Ultimately, understanding and applying the correct standards enables organizations to create QR code experiences that are trustworthy, secure, and universally accessible, strengthening user confidence in this widely adopted technology.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C18" t="str">
         <v>admin</v>
@@ -1203,12 +1574,37 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" xml:space="preserve">
       <c r="A19" t="str">
         <v>QR Codes in Travel and Tourism</v>
       </c>
-      <c r="B19" t="str">
-        <v>&lt;h1&gt;QR Codes in Travel and Tourism&lt;/h1&gt;&lt;p&gt;The travel industry has embraced QR codes to streamline processes and enhance tourist experiences.&lt;/p&gt;&lt;h2&gt;Travel Applications&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Digital boarding passes&lt;/li&gt;&lt;li&gt;Hotel check-in systems&lt;/li&gt;&lt;li&gt;Tourist information points&lt;/li&gt;&lt;li&gt;Restaurant menus and ordering&lt;/li&gt;&lt;li&gt;Museum and attraction guides&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Benefits for Travelers&lt;/h2&gt;&lt;p&gt;QR codes reduce paperwork, minimize language barriers, and provide instant access to information and services.&lt;/p&gt;</v>
+      <c r="B19" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article lang="en"&gt;
+  &lt;p&gt;
+    In today’s fast-evolving digital landscape, &lt;strong&gt;QR codes&lt;/strong&gt; have become a transformative tool within the &lt;strong&gt;travel and tourism industry&lt;/strong&gt;. Their ability to connect physical destinations with digital experiences has reshaped the way travelers access information, navigate locations, and engage with tourism services. As a result, QR codes are no longer just a convenience—they are a strategic technology that enhances efficiency, personalization, and customer satisfaction across the sector.
+  &lt;/p&gt;
+  &lt;p&gt;
+    One of the most significant benefits of QR codes in tourism is their role in providing &lt;strong&gt;contactless information access&lt;/strong&gt;. Travelers can quickly scan a QR code to view digital brochures, tour details, or cultural insights without touching shared materials. This became particularly important during the global pandemic, but the convenience and hygiene advantages continue to drive widespread adoption. By replacing printed guides with dynamic digital content, organizations can also reduce costs and environmental impact.
+  &lt;/p&gt;
+  &lt;p&gt;
+    QR codes also enhance the &lt;strong&gt;visitor experience&lt;/strong&gt; at historical sites, museums, and natural attractions. Instead of static plaques with limited space, QR-driven digital guides can offer rich multimedia experiences, including videos, audio tours, high-resolution images, and multi-language descriptions. This allows tourists to explore destinations at their own pace and in their preferred language, creating a more engaging and inclusive experience. For tourism boards, this added layer of interactivity strengthens destination branding and visitor satisfaction.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Navigation is another key area where QR codes provide value. Travelers can scan codes positioned at transportation hubs, public squares, and tourist hotspots to access &lt;strong&gt;real-time maps&lt;/strong&gt;, transit schedules, and walking routes. Deep linking capabilities allow QR codes to open apps with preloaded location data, simplifying navigation even for visitors unfamiliar with the area. This reduces confusion, enhances safety, and improves the overall travel experience.
+  &lt;/p&gt;
+  &lt;p&gt;
+    A growing application of QR codes in travel is the facilitation of &lt;strong&gt;smart ticketing&lt;/strong&gt;. Airlines, train companies, and event organizers use QR-based tickets to streamline check-in and entry processes. Digital tickets reduce waiting times, eliminate the need for paper prints, and enhance security through unique, scannable identifiers. Hotels also benefit from QR codes by allowing guests to access &lt;strong&gt;digital menus&lt;/strong&gt;, room service options, Wi-Fi login pages, and local recommendations instantly.
+  &lt;/p&gt;
+  &lt;p&gt;
+    For tourism operators, QR codes offer significant advantages in terms of &lt;strong&gt;marketing and analytics&lt;/strong&gt;. By tracking scan data, businesses can understand visitor behavior, determine popular attractions, and evaluate the effectiveness of promotional campaigns. QR codes placed in different locations can help identify which areas draw the most engagement, enabling data-driven decision-making. This insight allows tourism agencies to improve services, optimize resource allocation, and tailor experiences to traveler preferences.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Another powerful use case is the integration of QR codes with &lt;strong&gt;local businesses&lt;/strong&gt;. Restaurants, souvenir shops, and tour operators can use QR codes to offer special discounts, promote loyalty programs, or display multilingual menus. This strengthens the connection between travelers and local economies by increasing visibility and accessibility. QR-driven promotions can also be updated instantly, allowing businesses to adapt to seasonal trends or visitor demands without reprinting materials.
+  &lt;/p&gt;
+  &lt;p&gt;
+    In conclusion, QR codes have become an essential component of modern travel and tourism. Their ability to deliver &lt;strong&gt;instant information&lt;/strong&gt;, enhance navigation, support contactless experiences, and provide valuable analytics makes them a powerful tool for both travelers and tourism organizations. As digital transformation continues to shape the industry, the use of QR codes will only expand, driving greater innovation and more personalized travel experiences. By embracing this versatile technology, destinations can create smarter, more connected tourism ecosystems that benefit visitors and businesses alike.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C19" t="str">
         <v>admin</v>
@@ -1247,12 +1643,37 @@
         <v>Blogs</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" xml:space="preserve">
       <c r="A20" t="str">
         <v>QR Code Analytics: Measuring Success</v>
       </c>
-      <c r="B20" t="str">
-        <v>&lt;h1&gt;QR Code Analytics&lt;/h1&gt;&lt;p&gt;Understanding QR code performance metrics is essential for optimizing campaigns and measuring ROI.&lt;/p&gt;&lt;h2&gt;Key Metrics&lt;/h2&gt;&lt;ul&gt;&lt;li&gt;Scan count and frequency&lt;/li&gt;&lt;li&gt;Geographic distribution&lt;/li&gt;&lt;li&gt;Device and platform data&lt;/li&gt;&lt;li&gt;Time-based patterns&lt;/li&gt;&lt;/ul&gt;&lt;h2&gt;Optimization Strategies&lt;/h2&gt;&lt;p&gt;By analyzing scan data, businesses can refine placement, design, and content to improve engagement rates.&lt;/p&gt;</v>
+      <c r="B20" t="str" xml:space="preserve">
+        <v xml:space="preserve">&lt;article lang="en"&gt;
+  &lt;p&gt;
+    As QR codes continue to grow in popularity across industries—from retail and advertising to logistics and event management—the ability to measure their performance has become essential. QR code analytics provide valuable insights into user behavior, campaign success, and overall engagement. By analyzing these data points, businesses can refine their strategies, allocate budgets more effectively, and create more personalized user experiences. Understanding QR code analytics is no longer optional; it is a key component of any data-driven digital initiative.
+  &lt;/p&gt;
+  &lt;p&gt;
+    One of the primary metrics used in QR code analytics is the number of scans. Scan counts reveal how many people interacted with a particular QR code, highlighting the effectiveness of placement, design, and messaging. However, scan counts alone do not provide a complete picture. Advanced analytics platforms offer additional details such as unique scans versus repeat scans, giving businesses deeper insights into user interest and engagement quality. For example, a high number of repeat scans may indicate strong curiosity or the need for repeated access to the same resource.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Another crucial aspect of QR code analytics is geographical data. This information identifies the locations where QR codes are most frequently scanned, allowing businesses to detect regional trends or assess the performance of localized campaigns. For global brands, geographic insights can guide market expansion, refine advertising placement, and optimize regional content strategies. Even for small businesses, understanding local engagement can shape decisions about where to distribute promotional materials or where customer interest is strongest.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Device and operating system data are also important in measuring QR code success. Analytics platforms often track whether users scan codes using Android or iOS devices, as well as whether they use built-in camera apps or third-party QR readers. These insights help developers and marketers ensure that landing pages, apps, or content linked to QR codes are optimized across devices. Additionally, technical data can inform whether certain features, such as deep linking or app-specific redirects, are functioning as intended.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Time-based performance metrics provide another layer of insight. By analyzing the days and hours when QR codes are scanned most frequently, businesses can identify patterns in user engagement. This information can be used to schedule advertisements, send push notifications, or launch time-sensitive promotions strategically. Seasonal or event-based peaks may also emerge, giving organizations the ability to capitalize on specific moments when users are most receptive.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Engagement quality beyond the scan is equally important. Many advanced QR code systems track user behavior after the scan—such as how long users stay on the landing page, what buttons they click, or whether they complete a purchase or form submission. These post-scan interactions provide measurable indicators of conversion performance. By connecting QR codes to analytics tools like Google Analytics or mobile app dashboards, businesses can follow the entire user journey from physical interaction to digital action.
+  &lt;/p&gt;
+  &lt;p&gt;
+    Ultimately, the purpose of QR code analytics is not just to collect data, but to translate it into actionable insights. Businesses can A/B test different QR code designs, CTAs, or placements to determine what drives the highest engagement. They can personalize experiences based on geographic or demographic trends or improve app onboarding flows by analyzing where users drop off. With the right analytical framework, QR codes become powerful instruments that support continuous optimization and measurable growth.
+  &lt;/p&gt;
+  &lt;p&gt;
+    In conclusion, QR code analytics are essential for understanding user engagement and evaluating campaign effectiveness. By tracking metrics such as scan volume, location, device type, and post-scan behavior, businesses gain a holistic view of how their QR initiatives perform. As QR technology becomes even more integrated into mobile apps and physical environments, the ability to interpret these metrics will continue to provide a competitive advantage. Carefully analyzing and applying these insights ensures that QR-driven strategies deliver meaningful results and long-term value.
+  &lt;/p&gt;
+&lt;/article&gt;</v>
       </c>
       <c r="C20" t="str">
         <v>admin</v>

</xml_diff>